<commit_message>
fixed typo for Fig 3di Supp Fig4j dataset
</commit_message>
<xml_diff>
--- a/input_data/list_of_RAWdatasets.xlsx
+++ b/input_data/list_of_RAWdatasets.xlsx
@@ -50596,7 +50596,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>531</v>
@@ -50613,7 +50613,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>532</v>
@@ -50630,7 +50630,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>533</v>
@@ -50647,7 +50647,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>534</v>
@@ -50664,7 +50664,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>535</v>
@@ -50681,7 +50681,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>536</v>
@@ -50698,7 +50698,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>537</v>
@@ -50715,7 +50715,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>538</v>
@@ -50732,7 +50732,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>539</v>
@@ -50749,7 +50749,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>540</v>
@@ -50766,7 +50766,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
         <v>541</v>
@@ -50783,7 +50783,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
         <v>542</v>

</xml_diff>